<commit_message>
Updated path bug in tests
</commit_message>
<xml_diff>
--- a/test/assets/Book1.xlsx
+++ b/test/assets/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
   </bookViews>
@@ -575,6 +575,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -587,6 +588,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -599,5 +601,6 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>